<commit_message>
adding formulas to Excel output
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/sensedComp2.xlsx
+++ b/shipClassTests/testResults/sensedComp2.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sensed Comp2_LR History" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensed Comp2_LR" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -362,9 +362,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="12.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1">
+        <f>MODE(C[100, 0, 0, 3] : C[100, 0, 0, 3])</f>
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -413,7 +417,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -427,7 +431,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -441,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -606,7 +610,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -620,7 +624,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -634,7 +638,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -648,7 +652,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -662,7 +666,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -676,7 +680,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -690,7 +694,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -704,7 +708,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -718,7 +722,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -732,7 +736,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -746,7 +750,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -760,7 +764,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -774,7 +778,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -788,7 +792,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -802,7 +806,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -816,7 +820,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -830,7 +834,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1113,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54">
         <v>3</v>
@@ -1127,7 +1131,7 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
         <v>3</v>
@@ -1141,7 +1145,7 @@
         <v>3</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56">
         <v>3</v>
@@ -1306,7 +1310,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -1320,7 +1324,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -1334,7 +1338,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -1348,7 +1352,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -1362,7 +1366,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -1376,7 +1380,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -1390,7 +1394,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -1404,7 +1408,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -1418,7 +1422,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -1432,7 +1436,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -1446,7 +1450,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -1460,7 +1464,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -1474,7 +1478,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -1488,7 +1492,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -1502,7 +1506,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -1516,7 +1520,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -1530,7 +1534,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C84">
         <v>0</v>

</xml_diff>